<commit_message>
adjusted config reading and first try of readme
</commit_message>
<xml_diff>
--- a/SatelliteSimulation/config.xlsx
+++ b/SatelliteSimulation/config.xlsx
@@ -1,19 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombr\OneDrive\Dokumente\Privat\Uni\HWR\5.FS\Studienprojekt II\studienProjekt2\SatelliteSimulation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD334636-BDEE-4A0A-932E-27EE43B3FB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>SatelliteA</t>
+  </si>
+  <si>
+    <t>SatelliteB</t>
+  </si>
+  <si>
+    <t>SatelliteC</t>
+  </si>
+  <si>
+    <t>SatelliteD</t>
+  </si>
+  <si>
+    <t>observance-radius [0-300]</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -21,13 +55,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -42,14 +95,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,43 +441,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>SatelliteA</v>
-      </c>
-      <c r="B1" t="str">
-        <v>SatelliteB</v>
-      </c>
-      <c r="C1" t="str">
-        <v>SatelliteC</v>
-      </c>
-      <c r="D1" t="str">
-        <v>SatelliteD</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
         <v>100</v>
       </c>
-      <c r="B2" t="str">
-        <v>100</v>
-      </c>
-      <c r="C2" t="str">
-        <v>100</v>
-      </c>
-      <c r="D2" t="str">
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3">
         <v>100</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="K2QKZyCH7tn9cwVr0oyWSGmGq/eEODUP3m6az2NFyU9HhBQf98kb3y1be556yPooKcsrH6inZLtB0ezefUppJw==" saltValue="z/bne3tmZDyoMAjnauoFRA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError sqref="A1:E1 A2 C2:D2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>